<commit_message>
Added stage name column to sorghum harvesting observations
Need to check if these stage names are correct...some of the stage numbers are odd.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/Observed.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ApsimX\Prototypes\Sorghum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\UnderReview\Sorghum\obs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3C946A-5382-4774-93CA-99FE7623D8F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D261E2-0186-4B9E-8BE3-0E92ADCEA9C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51600" yWindow="300" windowWidth="24930" windowHeight="19710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="161">
   <si>
     <t>Experiment</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>Sorghum_BW8_GxE_T9</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>HarvestRipe</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO83"/>
+  <dimension ref="A1:AP83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1321,7 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -1439,8 +1445,11 @@
       <c r="AO1" t="s">
         <v>38</v>
       </c>
+      <c r="AP1" t="s">
+        <v>159</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1555,8 +1564,11 @@
       <c r="AO2">
         <v>3840.77</v>
       </c>
+      <c r="AP2" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1674,8 +1686,11 @@
       <c r="AO3">
         <v>3375.09</v>
       </c>
+      <c r="AP3" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1793,8 +1808,11 @@
       <c r="AO4">
         <v>4436.9399999999996</v>
       </c>
+      <c r="AP4" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1900,8 +1918,11 @@
       <c r="AO5">
         <v>2907.07</v>
       </c>
+      <c r="AP5" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2013,8 +2034,11 @@
       <c r="AO6">
         <v>2228.56</v>
       </c>
+      <c r="AP6" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2126,8 +2150,11 @@
       <c r="AO7">
         <v>3167.19</v>
       </c>
+      <c r="AP7" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2242,8 +2269,11 @@
       <c r="AO8">
         <v>3075.96</v>
       </c>
+      <c r="AP8" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2358,8 +2388,11 @@
       <c r="AO9">
         <v>2667.13</v>
       </c>
+      <c r="AP9" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2441,8 +2474,11 @@
       <c r="AO10">
         <v>2687.43</v>
       </c>
+      <c r="AP10" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2554,8 +2590,11 @@
       <c r="AO11">
         <v>2992.66</v>
       </c>
+      <c r="AP11" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2670,8 +2709,11 @@
       <c r="AO12">
         <v>2724.6</v>
       </c>
+      <c r="AP12" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -2786,8 +2828,11 @@
       <c r="AO13">
         <v>2347.0500000000002</v>
       </c>
+      <c r="AP13" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2905,8 +2950,11 @@
       <c r="AO14">
         <v>4258.07</v>
       </c>
+      <c r="AP14" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -3027,8 +3075,11 @@
       <c r="AO15">
         <v>5864.85</v>
       </c>
+      <c r="AP15" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -3149,8 +3200,11 @@
       <c r="AO16">
         <v>7226.11</v>
       </c>
+      <c r="AP16" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -3262,8 +3316,11 @@
       <c r="AO17">
         <v>4004.71</v>
       </c>
+      <c r="AP17" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -3381,8 +3438,11 @@
       <c r="AO18">
         <v>4351.74</v>
       </c>
+      <c r="AP18" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -3500,8 +3560,11 @@
       <c r="AO19">
         <v>4571.74</v>
       </c>
+      <c r="AP19" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -3619,8 +3682,11 @@
       <c r="AO20">
         <v>3374.77</v>
       </c>
+      <c r="AP20" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -3705,8 +3771,11 @@
       <c r="AO21">
         <v>3712.15</v>
       </c>
+      <c r="AP21" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -3803,8 +3872,11 @@
       <c r="AO22">
         <v>4769.57</v>
       </c>
+      <c r="AP22" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -3922,8 +3994,11 @@
       <c r="AO23">
         <v>3480.9</v>
       </c>
+      <c r="AP23" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -4008,8 +4083,11 @@
       <c r="AO24">
         <v>3280.66</v>
       </c>
+      <c r="AP24" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -4106,8 +4184,11 @@
       <c r="AO25">
         <v>4838.2299999999996</v>
       </c>
+      <c r="AP25" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -4174,8 +4255,11 @@
       <c r="AO26">
         <v>3357.92</v>
       </c>
+      <c r="AP26" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -4242,8 +4326,11 @@
       <c r="AO27">
         <v>2441.16</v>
       </c>
+      <c r="AP27" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -4310,8 +4397,11 @@
       <c r="AO28">
         <v>1980.81</v>
       </c>
+      <c r="AP28" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -4378,8 +4468,11 @@
       <c r="AO29">
         <v>1743.25</v>
       </c>
+      <c r="AP29" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -4446,8 +4539,11 @@
       <c r="AO30">
         <v>3960.09</v>
       </c>
+      <c r="AP30" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -4514,8 +4610,11 @@
       <c r="AO31">
         <v>2718</v>
       </c>
+      <c r="AP31" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -4582,8 +4681,11 @@
       <c r="AO32">
         <v>2589.62</v>
       </c>
+      <c r="AP32" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -4650,8 +4752,11 @@
       <c r="AO33">
         <v>3334.48</v>
       </c>
+      <c r="AP33" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -4718,8 +4823,11 @@
       <c r="AO34">
         <v>3530.61</v>
       </c>
+      <c r="AP34" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -4786,8 +4894,11 @@
       <c r="AO35">
         <v>2926.94</v>
       </c>
+      <c r="AP35" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -4854,8 +4965,11 @@
       <c r="AO36">
         <v>2272.98</v>
       </c>
+      <c r="AP36" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -4922,8 +5036,11 @@
       <c r="AO37">
         <v>2640.16</v>
       </c>
+      <c r="AP37" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -4990,8 +5107,11 @@
       <c r="AO38">
         <v>3114.52</v>
       </c>
+      <c r="AP38" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -5058,8 +5178,11 @@
       <c r="AO39">
         <v>2971.98</v>
       </c>
+      <c r="AP39" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -5126,8 +5249,11 @@
       <c r="AO40">
         <v>2095.77</v>
       </c>
+      <c r="AP40" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -5194,8 +5320,11 @@
       <c r="AO41">
         <v>1873.2</v>
       </c>
+      <c r="AP41" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -5262,8 +5391,11 @@
       <c r="AO42">
         <v>3470.54</v>
       </c>
+      <c r="AP42" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -5330,8 +5462,11 @@
       <c r="AO43">
         <v>2197.9499999999998</v>
       </c>
+      <c r="AP43" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -5398,8 +5533,11 @@
       <c r="AO44">
         <v>2002.73</v>
       </c>
+      <c r="AP44" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>154</v>
       </c>
@@ -5466,8 +5604,11 @@
       <c r="AO45">
         <v>2797.17</v>
       </c>
+      <c r="AP45" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>155</v>
       </c>
@@ -5534,8 +5675,11 @@
       <c r="AO46">
         <v>3208</v>
       </c>
+      <c r="AP46" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -5602,8 +5746,11 @@
       <c r="AO47">
         <v>2267.75</v>
       </c>
+      <c r="AP47" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>157</v>
       </c>
@@ -5670,8 +5817,11 @@
       <c r="AO48">
         <v>1957.42</v>
       </c>
+      <c r="AP48" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>158</v>
       </c>
@@ -5738,8 +5888,11 @@
       <c r="AO49">
         <v>2720.84</v>
       </c>
+      <c r="AP49" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -5833,8 +5986,11 @@
       <c r="AO50">
         <v>4070.29</v>
       </c>
+      <c r="AP50" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -5928,8 +6084,11 @@
       <c r="AO51">
         <v>3548.66</v>
       </c>
+      <c r="AP51" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -6023,8 +6182,11 @@
       <c r="AO52">
         <v>3312.67</v>
       </c>
+      <c r="AP52" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -6118,8 +6280,11 @@
       <c r="AO53">
         <v>2601.52</v>
       </c>
+      <c r="AP53" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -6213,8 +6378,11 @@
       <c r="AO54">
         <v>3047.26</v>
       </c>
+      <c r="AP54" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -6308,8 +6476,11 @@
       <c r="AO55">
         <v>2445.31</v>
       </c>
+      <c r="AP55" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -6397,8 +6568,11 @@
       <c r="AO56">
         <v>3636.92</v>
       </c>
+      <c r="AP56" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>113</v>
       </c>
@@ -6486,8 +6660,11 @@
       <c r="AO57">
         <v>4869.21</v>
       </c>
+      <c r="AP57" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>115</v>
       </c>
@@ -6575,8 +6752,11 @@
       <c r="AO58">
         <v>4427.03</v>
       </c>
+      <c r="AP58" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -6661,8 +6841,11 @@
       <c r="AO59">
         <v>3710.9</v>
       </c>
+      <c r="AP59" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -6747,8 +6930,11 @@
       <c r="AO60">
         <v>4815.8500000000004</v>
       </c>
+      <c r="AP60" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -6833,8 +7019,11 @@
       <c r="AO61">
         <v>3898.34</v>
       </c>
+      <c r="AP61" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>121</v>
       </c>
@@ -6901,8 +7090,11 @@
       <c r="AO62">
         <v>2788.91</v>
       </c>
+      <c r="AP62" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -6969,8 +7161,11 @@
       <c r="AO63">
         <v>2556.4899999999998</v>
       </c>
+      <c r="AP63" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -7046,8 +7241,11 @@
       <c r="AO64">
         <v>4245.6099999999997</v>
       </c>
+      <c r="AP64" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -7123,8 +7321,11 @@
       <c r="AO65">
         <v>4188.6099999999997</v>
       </c>
+      <c r="AP65" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -7200,8 +7401,11 @@
       <c r="AO66">
         <v>5248.38</v>
       </c>
+      <c r="AP66" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -7286,8 +7490,11 @@
       <c r="AO67">
         <v>1242</v>
       </c>
+      <c r="AP67" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>129</v>
       </c>
@@ -7372,8 +7579,11 @@
       <c r="AO68">
         <v>1302.6600000000001</v>
       </c>
+      <c r="AP68" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>130</v>
       </c>
@@ -7458,8 +7668,11 @@
       <c r="AO69">
         <v>1407.88</v>
       </c>
+      <c r="AP69" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>131</v>
       </c>
@@ -7544,8 +7757,11 @@
       <c r="AO70">
         <v>1247.05</v>
       </c>
+      <c r="AP70" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>132</v>
       </c>
@@ -7630,8 +7846,11 @@
       <c r="AO71">
         <v>2498.5</v>
       </c>
+      <c r="AP71" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -7716,8 +7935,11 @@
       <c r="AO72">
         <v>1197</v>
       </c>
+      <c r="AP72" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>134</v>
       </c>
@@ -7802,8 +8024,11 @@
       <c r="AO73">
         <v>2168.06</v>
       </c>
+      <c r="AP73" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>135</v>
       </c>
@@ -7888,8 +8113,11 @@
       <c r="AO74">
         <v>1973.5</v>
       </c>
+      <c r="AP74" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -7962,8 +8190,11 @@
       <c r="AO75">
         <v>4896.1000000000004</v>
       </c>
+      <c r="AP75" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>138</v>
       </c>
@@ -8036,8 +8267,11 @@
       <c r="AO76">
         <v>4159.84</v>
       </c>
+      <c r="AP76" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>139</v>
       </c>
@@ -8110,8 +8344,11 @@
       <c r="AO77">
         <v>3767.5</v>
       </c>
+      <c r="AP77" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>140</v>
       </c>
@@ -8184,8 +8421,11 @@
       <c r="AO78">
         <v>5175.38</v>
       </c>
+      <c r="AP78" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>141</v>
       </c>
@@ -8258,8 +8498,11 @@
       <c r="AO79">
         <v>4488.97</v>
       </c>
+      <c r="AP79" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>142</v>
       </c>
@@ -8332,8 +8575,11 @@
       <c r="AO80">
         <v>4175.2299999999996</v>
       </c>
+      <c r="AP80" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>143</v>
       </c>
@@ -8406,8 +8652,11 @@
       <c r="AO81">
         <v>5689.22</v>
       </c>
+      <c r="AP81" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>144</v>
       </c>
@@ -8480,8 +8729,11 @@
       <c r="AO82">
         <v>4516.24</v>
       </c>
+      <c r="AP82" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>145</v>
       </c>
@@ -8553,6 +8805,9 @@
       </c>
       <c r="AO83">
         <v>4018.63</v>
+      </c>
+      <c r="AP83" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>